<commit_message>
Metric conversions of the respective parts.
</commit_message>
<xml_diff>
--- a/Metric Modifications/Replacement_COTS.xlsx
+++ b/Metric Modifications/Replacement_COTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/home/github/OpenHornet-metric/Metric Modifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCB81ED-955C-5F4D-8A48-6CE5C18D9421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACCDD32-4686-994A-929D-9AFBC8870FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" xr2:uid="{D93EFF7A-6B33-AC4D-9A9C-C443CD52EB89}"/>
   </bookViews>
@@ -42,7 +42,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="3">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -57,30 +57,20 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="3">
+  <valueMetadata count="2">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
     </bk>
-    <bk>
-      <rc t="1" v="2"/>
-    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
   <si>
     <t>Abmessungen Imperial</t>
   </si>
@@ -472,9 +462,6 @@
     <t>https://www.amazon.de/dp/B09QX3THX3?ref=ppx_yo2ov_dt_b_product_details&amp;th=1</t>
   </si>
   <si>
-    <t>https://www.amazon.de/Universalschraube-Senkkopf-schwarz-T-STAR-Vollgewinde/dp/B09QXDLVB6?ref_=ast_sto_dp&amp;th=1</t>
-  </si>
-  <si>
     <t>4 mm x 40 mm</t>
   </si>
   <si>
@@ -523,16 +510,25 @@
     <t>https://www.amazon.de/gp/product/B09FXNLYTN/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;th=1</t>
   </si>
   <si>
-    <t>M2,5 x 4</t>
-  </si>
-  <si>
-    <t>https://www.amazon.de/gp/product/B09J91JWGM/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gewindeeinsatz 6-32 für Kunststiff. Höhe ca. </t>
   </si>
   <si>
     <t>6-32</t>
+  </si>
+  <si>
+    <t>Lochdurchmesser 5,6 mm</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/Universalschraube-Senkkopf-schwarz-T-STAR-Vollgewinde/dp/B09QX782N9?ref_=ast_sto_dp&amp;th=1</t>
+  </si>
+  <si>
+    <t>M2,5 x 4 // M2 x 3</t>
+  </si>
+  <si>
+    <t>M2 x 3 besser wegen Platzbedarf der Mutter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/gp/product/B0BG16KFTM/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -726,17 +722,13 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <v>0</v>
     <v>5</v>
   </rv>
   <rv s="0">
     <v>1</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -755,7 +747,6 @@
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
   <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -1059,7 +1050,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1153,7 @@
         <v>52</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1179,7 +1170,7 @@
         <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -1193,7 +1184,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -1219,7 +1210,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1239,7 +1230,7 @@
         <v>11</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1259,7 +1250,7 @@
         <v>77</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1279,7 +1270,7 @@
         <v>74</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1305,7 +1296,7 @@
         <v>125</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -1328,7 +1319,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -1353,10 +1344,10 @@
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1370,10 +1361,10 @@
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,13 +1378,13 @@
         <v>18</v>
       </c>
       <c r="E30" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="G30" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1401,13 +1392,13 @@
         <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G31" t="s">
         <v>125</v>
@@ -1424,10 +1415,13 @@
         <v>126</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="G32" t="s">
+        <v>151</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1435,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>73</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,7 +1472,7 @@
       <c r="B43" t="s">
         <v>75</v>
       </c>
-      <c r="G43" t="e" vm="3">
+      <c r="G43" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1486,18 +1480,16 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H10" r:id="rId1" xr:uid="{CE876507-9B7C-564E-B359-6ED3413B92F4}"/>
-    <hyperlink ref="H9" r:id="rId2" xr:uid="{D1A4AD6F-4C61-684A-90B6-1A2B90B6E631}"/>
-    <hyperlink ref="H18" r:id="rId3" xr:uid="{BD467FBF-2E0F-084F-9405-2EA43A3401AB}"/>
-    <hyperlink ref="H17" r:id="rId4" xr:uid="{781EFB5D-65E1-5D48-B35F-42D7261F586B}"/>
-    <hyperlink ref="H16" r:id="rId5" xr:uid="{81D71EA9-16F4-C04D-8F25-E6FB71AAFC5C}"/>
-    <hyperlink ref="H14" r:id="rId6" xr:uid="{F0FAE1DF-FF7D-0648-B002-74A434BCC67F}"/>
-    <hyperlink ref="H13" r:id="rId7" xr:uid="{83ED10DD-6AC8-484A-B155-8D4DC00CE070}"/>
-    <hyperlink ref="H19" r:id="rId8" xr:uid="{2C31950A-0717-DA4F-9CEB-905802C9CDBC}"/>
-    <hyperlink ref="H22" r:id="rId9" xr:uid="{16693DBE-83F3-9841-ACAE-4C0D7D929DB3}"/>
-    <hyperlink ref="H23" r:id="rId10" xr:uid="{EC1C5360-3941-DB40-A532-FAAB949DDCEC}"/>
-    <hyperlink ref="H34" r:id="rId11" xr:uid="{0C1DF67D-7093-7F45-84C8-917306477800}"/>
-    <hyperlink ref="H30" r:id="rId12" xr:uid="{A8A6B72D-0ED1-874E-9AC8-C0688EB233C6}"/>
-    <hyperlink ref="H32" r:id="rId13" xr:uid="{50C5DA00-B12E-8441-A2CC-3CB8B76C48EA}"/>
+    <hyperlink ref="H18" r:id="rId2" xr:uid="{BD467FBF-2E0F-084F-9405-2EA43A3401AB}"/>
+    <hyperlink ref="H17" r:id="rId3" xr:uid="{781EFB5D-65E1-5D48-B35F-42D7261F586B}"/>
+    <hyperlink ref="H16" r:id="rId4" xr:uid="{81D71EA9-16F4-C04D-8F25-E6FB71AAFC5C}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{F0FAE1DF-FF7D-0648-B002-74A434BCC67F}"/>
+    <hyperlink ref="H13" r:id="rId6" xr:uid="{83ED10DD-6AC8-484A-B155-8D4DC00CE070}"/>
+    <hyperlink ref="H19" r:id="rId7" xr:uid="{2C31950A-0717-DA4F-9CEB-905802C9CDBC}"/>
+    <hyperlink ref="H22" r:id="rId8" xr:uid="{16693DBE-83F3-9841-ACAE-4C0D7D929DB3}"/>
+    <hyperlink ref="H23" r:id="rId9" xr:uid="{EC1C5360-3941-DB40-A532-FAAB949DDCEC}"/>
+    <hyperlink ref="H34" r:id="rId10" xr:uid="{0C1DF67D-7093-7F45-84C8-917306477800}"/>
+    <hyperlink ref="H30" r:id="rId11" xr:uid="{A8A6B72D-0ED1-874E-9AC8-C0688EB233C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test.md gelöscht, weil nur Testdatei
</commit_message>
<xml_diff>
--- a/Metric Modifications/Replacement_COTS.xlsx
+++ b/Metric Modifications/Replacement_COTS.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/home/github/OpenHornet-metric/Metric Modifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F347C65-4561-7F4E-AF9A-FA8FCA81C346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D320122-BE65-8443-960C-B204F3208D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="3" xr2:uid="{D93EFF7A-6B33-AC4D-9A9C-C443CD52EB89}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" xr2:uid="{D93EFF7A-6B33-AC4D-9A9C-C443CD52EB89}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ersatzartikel" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Zoll - metrisch" sheetId="3" r:id="rId3"/>
     <sheet name="Gravurmaterial" sheetId="4" r:id="rId4"/>
     <sheet name="Schraubenquellen" sheetId="5" r:id="rId5"/>
     <sheet name="Aufbau Panels" sheetId="6" r:id="rId6"/>
-    <sheet name="Tabelle7" sheetId="7" r:id="rId7"/>
+    <sheet name="Schraubenlager" sheetId="8" r:id="rId7"/>
+    <sheet name="MDF lackieren" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="884">
   <si>
     <t>M4 x 30 mm</t>
   </si>
@@ -2184,36 +2185,6 @@
     <t>3,505 x  31,75 mm</t>
   </si>
   <si>
-    <t>DIN 7991, ISO 10643</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10644</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10645</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10646</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10647</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10648</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10649</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10650</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10651</t>
-  </si>
-  <si>
-    <t>DIN 7991, ISO 10652</t>
-  </si>
-  <si>
     <t>DIN 7991, ISO 10642; alternativ DIN14581 (Torx)</t>
   </si>
   <si>
@@ -2593,6 +2564,159 @@
   </si>
   <si>
     <t>12,90 € + MwSt.</t>
+  </si>
+  <si>
+    <t>SET SCREW, 8-32 X .125, CUP POINT, 18-8</t>
+  </si>
+  <si>
+    <t>4,166 mm x 3,175 mm</t>
+  </si>
+  <si>
+    <t>M4 x 3 mm</t>
+  </si>
+  <si>
+    <t>4,166 mm x 4,7625 mm</t>
+  </si>
+  <si>
+    <t>4,166 mm x 7,9375 mm</t>
+  </si>
+  <si>
+    <t>M4 x 5 mm</t>
+  </si>
+  <si>
+    <t>M4 x 8 mm</t>
+  </si>
+  <si>
+    <t>4,826 mm x 6,35 mm</t>
+  </si>
+  <si>
+    <t>M5 x 6 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 4,7625 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 3,175 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 2,38125 mm</t>
+  </si>
+  <si>
+    <t>M3,5 x 6 mm</t>
+  </si>
+  <si>
+    <t>M3 x 2 mm</t>
+  </si>
+  <si>
+    <t>M5 x 10 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 15,88 mm</t>
+  </si>
+  <si>
+    <t>M2 x 16 mm</t>
+  </si>
+  <si>
+    <t>M2 x 18 mm</t>
+  </si>
+  <si>
+    <t>1,524 mm x 9,53 mm</t>
+  </si>
+  <si>
+    <t>M1,6 x 10 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 7,94 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 25,4 mm</t>
+  </si>
+  <si>
+    <t>3,505 mm x 3,175 mm</t>
+  </si>
+  <si>
+    <t>6,35 mm x 9,53 mm</t>
+  </si>
+  <si>
+    <t>6,35 mm x 19,05 mm</t>
+  </si>
+  <si>
+    <t>M6x 10 mm</t>
+  </si>
+  <si>
+    <t>M6 x 20 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 3,175 mm</t>
+  </si>
+  <si>
+    <t>M2x 3 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 4,76 mm</t>
+  </si>
+  <si>
+    <t>M2 x 5 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 9,525 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 38,1 mm</t>
+  </si>
+  <si>
+    <t>M2 x 40 mm</t>
+  </si>
+  <si>
+    <t>1,524 mm</t>
+  </si>
+  <si>
+    <t>Schraubenlager</t>
+  </si>
+  <si>
+    <t>2,5 mm</t>
+  </si>
+  <si>
+    <t>2 mm</t>
+  </si>
+  <si>
+    <t>3 mm</t>
+  </si>
+  <si>
+    <t>4 mm</t>
+  </si>
+  <si>
+    <t>5 mm</t>
+  </si>
+  <si>
+    <t>8 mm</t>
+  </si>
+  <si>
+    <t>10 mm</t>
+  </si>
+  <si>
+    <t>Linsenkopf</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Senkkopf</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Zylinderkopf</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Außensechskant</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2805,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2712,6 +2836,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2735,7 +2889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2773,6 +2927,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -3203,8 +3371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B20728A-6C41-1849-BB83-42D2A465FBDB}">
   <dimension ref="A1:J311"/>
   <sheetViews>
-    <sheetView topLeftCell="C184" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J210" sqref="J210"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,11 +3794,11 @@
       <c r="B24" s="16" t="s">
         <v>643</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="29">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>651</v>
@@ -3649,7 +3817,7 @@
       <c r="B25" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="29">
         <v>4</v>
       </c>
       <c r="D25" t="s">
@@ -3879,7 +4047,7 @@
       <c r="B37" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <v>13</v>
       </c>
       <c r="D37" t="s">
@@ -3902,7 +4070,7 @@
       <c r="B38" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <v>2</v>
       </c>
       <c r="D38" t="s">
@@ -3925,7 +4093,7 @@
       <c r="B39" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <v>11</v>
       </c>
       <c r="D39" t="s">
@@ -3948,7 +4116,7 @@
       <c r="B40" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="11">
         <v>16</v>
       </c>
       <c r="D40" t="s">
@@ -3971,7 +4139,7 @@
       <c r="B41" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="11">
         <v>2</v>
       </c>
       <c r="D41" t="s">
@@ -3983,7 +4151,7 @@
       <c r="F41" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="21" t="s">
         <v>678</v>
       </c>
     </row>
@@ -3994,7 +4162,7 @@
       <c r="B42" t="s">
         <v>229</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="11">
         <v>4</v>
       </c>
       <c r="D42" t="s">
@@ -4006,7 +4174,7 @@
       <c r="F42" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="21" t="s">
         <v>677</v>
       </c>
     </row>
@@ -4071,7 +4239,7 @@
         <v>285</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>716</v>
+        <v>706</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>668</v>
@@ -4111,10 +4279,10 @@
         <v>285</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="G49" s="17" t="s">
         <v>707</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4131,10 +4299,10 @@
         <v>285</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="G50" s="17" t="s">
         <v>708</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4151,7 +4319,7 @@
         <v>285</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>0</v>
@@ -4164,17 +4332,17 @@
       <c r="B52" t="s">
         <v>290</v>
       </c>
-      <c r="C52" s="12">
+      <c r="C52" s="23">
         <v>2</v>
       </c>
       <c r="D52" t="s">
         <v>285</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="G52" t="s">
-        <v>719</v>
+        <v>709</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4191,7 +4359,7 @@
         <v>285</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>4</v>
@@ -4211,10 +4379,10 @@
         <v>285</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>720</v>
+        <v>710</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -4231,10 +4399,10 @@
         <v>285</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>721</v>
+        <v>711</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -4251,10 +4419,10 @@
         <v>285</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>722</v>
+        <v>712</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -4271,10 +4439,10 @@
         <v>285</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="G57" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -4298,7 +4466,7 @@
         <v>101</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="G60" s="17" t="s">
         <v>65</v>
@@ -4347,7 +4515,7 @@
         <v>77</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="G62" s="17" t="s">
         <v>4</v>
@@ -4366,7 +4534,7 @@
       <c r="B63" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="12">
+      <c r="C63" s="23">
         <v>24</v>
       </c>
       <c r="D63" t="s">
@@ -4386,7 +4554,7 @@
       <c r="B64" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="23">
         <v>90</v>
       </c>
       <c r="D64" t="s">
@@ -4446,7 +4614,7 @@
       <c r="B68" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C68" s="12">
+      <c r="C68" s="29">
         <v>4</v>
       </c>
       <c r="D68" t="s">
@@ -4466,7 +4634,7 @@
       <c r="B69" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C69" s="12">
+      <c r="C69" s="29">
         <v>4</v>
       </c>
       <c r="D69" t="s">
@@ -4486,7 +4654,7 @@
       <c r="B70" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C70" s="12">
+      <c r="C70" s="29">
         <v>70</v>
       </c>
       <c r="D70" t="s">
@@ -4506,7 +4674,7 @@
       <c r="B71" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="18">
+      <c r="C71" s="30">
         <v>107</v>
       </c>
       <c r="D71" t="s">
@@ -4533,7 +4701,7 @@
       <c r="B72" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="C72" s="12">
+      <c r="C72" s="29">
         <v>2</v>
       </c>
       <c r="D72" t="s">
@@ -4553,7 +4721,7 @@
       <c r="B73" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="C73" s="12">
+      <c r="C73" s="29">
         <v>25</v>
       </c>
       <c r="D73" t="s">
@@ -4573,7 +4741,7 @@
       <c r="B74" s="16" t="s">
         <v>704</v>
       </c>
-      <c r="C74" s="12">
+      <c r="C74" s="29">
         <v>6</v>
       </c>
       <c r="D74" t="s">
@@ -4593,7 +4761,7 @@
       <c r="B75" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="C75" s="12">
+      <c r="C75" s="29">
         <v>5</v>
       </c>
       <c r="D75" t="s">
@@ -4726,7 +4894,7 @@
         <v>689</v>
       </c>
       <c r="G85" s="19" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -4736,11 +4904,17 @@
       <c r="B87" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="11">
         <v>4</v>
       </c>
       <c r="D87" t="s">
         <v>304</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="G87" s="16" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -4750,11 +4924,17 @@
       <c r="B89" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="11">
         <v>5</v>
       </c>
       <c r="D89" t="s">
         <v>304</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G89" s="16" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -4764,11 +4944,17 @@
       <c r="B90" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="11">
         <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>304</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -4778,11 +4964,17 @@
       <c r="B91" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="11">
         <v>27</v>
       </c>
       <c r="D91" t="s">
         <v>304</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="G91" s="16" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -4792,11 +4984,17 @@
       <c r="B92" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="11">
         <v>2</v>
       </c>
       <c r="D92" t="s">
         <v>304</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="G92" s="16" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -4806,7 +5004,7 @@
       <c r="B93" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="11">
         <v>11</v>
       </c>
       <c r="D93" t="s">
@@ -4814,6 +5012,9 @@
       </c>
       <c r="E93" s="1" t="s">
         <v>92</v>
+      </c>
+      <c r="G93" s="16" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -4823,11 +5024,17 @@
       <c r="B94" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C94" s="23">
         <v>22</v>
       </c>
       <c r="D94" t="s">
         <v>304</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="G94" s="16" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -4837,11 +5044,17 @@
       <c r="B95" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="23">
         <v>10</v>
       </c>
       <c r="D95" t="s">
         <v>304</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G95" s="16" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -4851,11 +5064,17 @@
       <c r="B96" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="23">
         <v>8</v>
       </c>
       <c r="D96" t="s">
         <v>304</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -4931,6 +5150,12 @@
       <c r="D102" t="s">
         <v>305</v>
       </c>
+      <c r="E102" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="G102" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
@@ -4997,7 +5222,7 @@
         <v>299</v>
       </c>
       <c r="G107" s="17" t="s">
-        <v>724</v>
+        <v>714</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -5014,7 +5239,7 @@
         <v>299</v>
       </c>
       <c r="G108" s="17" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -5048,7 +5273,7 @@
         <v>299</v>
       </c>
       <c r="G110" s="17" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -5058,11 +5283,14 @@
       <c r="B111" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C111" s="10">
+      <c r="C111" s="23">
         <v>10</v>
       </c>
       <c r="D111" t="s">
         <v>300</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>686</v>
       </c>
       <c r="G111" s="16" t="s">
         <v>667</v>
@@ -5075,14 +5303,17 @@
       <c r="B112" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C112" s="10">
+      <c r="C112" s="23">
         <v>2</v>
       </c>
       <c r="D112" t="s">
         <v>300</v>
       </c>
+      <c r="E112" s="1" t="s">
+        <v>855</v>
+      </c>
       <c r="G112" s="16" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5100,13 +5331,13 @@
         <v>326</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>331</v>
       </c>
       <c r="G114" s="17" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -5123,10 +5354,10 @@
         <v>326</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="G115" s="17" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -5143,10 +5374,10 @@
         <v>326</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>735</v>
+        <v>725</v>
       </c>
       <c r="G116" s="17" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -5163,10 +5394,10 @@
         <v>326</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="G117" s="17" t="s">
-        <v>739</v>
+        <v>729</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -5183,13 +5414,13 @@
         <v>327</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>328</v>
       </c>
       <c r="G118" s="17" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -5206,13 +5437,13 @@
         <v>330</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>329</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -5232,7 +5463,7 @@
         <v>331</v>
       </c>
       <c r="G121" s="17" t="s">
-        <v>728</v>
+        <v>718</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -5249,7 +5480,7 @@
         <v>326</v>
       </c>
       <c r="G122" s="17" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -5266,7 +5497,7 @@
         <v>326</v>
       </c>
       <c r="G123" s="17" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -5276,15 +5507,19 @@
       <c r="B125" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="C125" s="10">
+      <c r="C125" s="12">
         <v>4</v>
       </c>
       <c r="D125" t="s">
         <v>609</v>
       </c>
-      <c r="E125"/>
+      <c r="E125" t="s">
+        <v>654</v>
+      </c>
       <c r="F125"/>
-      <c r="G125" s="8"/>
+      <c r="G125" s="25" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -5293,14 +5528,19 @@
       <c r="B126" s="16" t="s">
         <v>470</v>
       </c>
-      <c r="C126" s="10">
+      <c r="C126" s="12">
         <v>2</v>
       </c>
       <c r="D126" t="s">
         <v>609</v>
       </c>
-      <c r="E126"/>
+      <c r="E126" t="s">
+        <v>853</v>
+      </c>
       <c r="F126"/>
+      <c r="G126" s="16" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
@@ -5309,14 +5549,19 @@
       <c r="B127" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="C127" s="10">
+      <c r="C127" s="12">
         <v>2</v>
       </c>
       <c r="D127" t="s">
         <v>609</v>
       </c>
-      <c r="E127"/>
+      <c r="E127" t="s">
+        <v>655</v>
+      </c>
       <c r="F127"/>
+      <c r="G127" s="16" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -5325,14 +5570,19 @@
       <c r="B128" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="C128" s="10">
+      <c r="C128" s="12">
         <v>9</v>
       </c>
       <c r="D128" t="s">
         <v>609</v>
       </c>
-      <c r="E128"/>
+      <c r="E128" t="s">
+        <v>854</v>
+      </c>
       <c r="F128"/>
+      <c r="G128" s="16" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -5341,14 +5591,19 @@
       <c r="B129" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="C129" s="10">
+      <c r="C129" s="12">
         <v>1</v>
       </c>
       <c r="D129" t="s">
         <v>609</v>
       </c>
-      <c r="E129"/>
+      <c r="E129" t="s">
+        <v>699</v>
+      </c>
       <c r="F129"/>
+      <c r="G129" s="16" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
@@ -5357,14 +5612,19 @@
       <c r="B130" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="C130" s="10">
+      <c r="C130" s="12">
         <v>4</v>
       </c>
       <c r="D130" t="s">
         <v>609</v>
       </c>
-      <c r="E130"/>
+      <c r="E130" t="s">
+        <v>856</v>
+      </c>
       <c r="F130"/>
+      <c r="G130" s="16" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
@@ -5373,14 +5633,19 @@
       <c r="B131" s="16" t="s">
         <v>480</v>
       </c>
-      <c r="C131" s="10">
+      <c r="C131" s="12">
         <v>4</v>
       </c>
       <c r="D131" t="s">
         <v>609</v>
       </c>
-      <c r="E131"/>
+      <c r="E131" t="s">
+        <v>857</v>
+      </c>
       <c r="F131"/>
+      <c r="G131" s="16" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -5398,7 +5663,7 @@
       <c r="E132"/>
       <c r="F132"/>
       <c r="G132" s="17" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -5419,7 +5684,7 @@
         <v>608</v>
       </c>
       <c r="G133" s="17" t="s">
-        <v>720</v>
+        <v>710</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -5436,11 +5701,11 @@
         <v>610</v>
       </c>
       <c r="E134" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
       <c r="F134"/>
       <c r="G134" s="17" t="s">
-        <v>749</v>
+        <v>739</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -5461,7 +5726,7 @@
       </c>
       <c r="F135"/>
       <c r="G135" s="17" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -5471,7 +5736,7 @@
       <c r="B136" t="s">
         <v>486</v>
       </c>
-      <c r="C136" s="12">
+      <c r="C136" s="23">
         <v>14</v>
       </c>
       <c r="D136" t="s">
@@ -5480,7 +5745,7 @@
       <c r="E136"/>
       <c r="F136"/>
       <c r="G136" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -5497,11 +5762,11 @@
         <v>610</v>
       </c>
       <c r="E137" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="F137"/>
       <c r="G137" s="17" t="s">
-        <v>748</v>
+        <v>738</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -5543,7 +5808,7 @@
         <v>612</v>
       </c>
       <c r="G139" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -5559,8 +5824,13 @@
       <c r="D140" t="s">
         <v>609</v>
       </c>
-      <c r="E140"/>
+      <c r="E140" t="s">
+        <v>860</v>
+      </c>
       <c r="F140"/>
+      <c r="G140" s="16" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="9" t="s">
@@ -5576,7 +5846,7 @@
         <v>625</v>
       </c>
       <c r="G143" s="17" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -5593,7 +5863,7 @@
         <v>626</v>
       </c>
       <c r="G144" s="19" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -5610,7 +5880,7 @@
         <v>627</v>
       </c>
       <c r="G145" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -5630,7 +5900,7 @@
         <v>645</v>
       </c>
       <c r="G146" s="18" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
@@ -5650,7 +5920,7 @@
         <v>74</v>
       </c>
       <c r="G147" s="17" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
@@ -5670,7 +5940,7 @@
         <v>628</v>
       </c>
       <c r="G148" s="17" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
@@ -5707,7 +5977,7 @@
         <v>644</v>
       </c>
       <c r="G150" s="17" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
@@ -5727,7 +5997,7 @@
         <v>645</v>
       </c>
       <c r="G151" s="17" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
@@ -5744,10 +6014,10 @@
         <v>631</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>758</v>
+        <v>748</v>
       </c>
       <c r="G152" s="17" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
@@ -5764,7 +6034,7 @@
         <v>625</v>
       </c>
       <c r="G153" s="17" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
@@ -5781,7 +6051,7 @@
         <v>625</v>
       </c>
       <c r="G154" s="17" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
@@ -5798,7 +6068,7 @@
         <v>625</v>
       </c>
       <c r="G155" s="17" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
@@ -5837,8 +6107,11 @@
       <c r="D157" t="s">
         <v>629</v>
       </c>
+      <c r="E157" s="1" t="s">
+        <v>867</v>
+      </c>
       <c r="G157" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
@@ -5852,13 +6125,13 @@
         <v>20</v>
       </c>
       <c r="D158" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>761</v>
+        <v>751</v>
       </c>
       <c r="G158" s="17" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
@@ -5872,10 +6145,10 @@
         <v>8</v>
       </c>
       <c r="D159" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="G159" s="17" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
@@ -5895,7 +6168,7 @@
         <v>630</v>
       </c>
       <c r="G160" s="17" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -5912,7 +6185,7 @@
         <v>631</v>
       </c>
       <c r="G161" s="17" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
@@ -5929,7 +6202,7 @@
         <v>631</v>
       </c>
       <c r="G162" s="17" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -5946,7 +6219,7 @@
         <v>631</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -5963,7 +6236,7 @@
         <v>631</v>
       </c>
       <c r="G164" s="17" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -5977,13 +6250,13 @@
         <v>39</v>
       </c>
       <c r="D165" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="G165" s="19" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="H165" t="s">
-        <v>788</v>
+        <v>778</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -6003,7 +6276,7 @@
         <v>74</v>
       </c>
       <c r="G166" s="17" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -6017,14 +6290,14 @@
         <v>46</v>
       </c>
       <c r="D168" t="s">
-        <v>767</v>
+        <v>757</v>
       </c>
       <c r="E168" t="s">
         <v>74</v>
       </c>
       <c r="F168"/>
       <c r="G168" s="21" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -6038,7 +6311,7 @@
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>780</v>
+        <v>770</v>
       </c>
       <c r="E169" t="s">
         <v>74</v>
@@ -6056,14 +6329,14 @@
         <v>4</v>
       </c>
       <c r="D170" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="F170"/>
       <c r="G170" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -6077,14 +6350,14 @@
         <v>12</v>
       </c>
       <c r="D171" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="F171"/>
       <c r="G171" t="s">
-        <v>773</v>
+        <v>763</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -6124,14 +6397,14 @@
         <v>8</v>
       </c>
       <c r="D174" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="E174"/>
       <c r="F174" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="G174" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -6145,14 +6418,14 @@
         <v>3</v>
       </c>
       <c r="D175" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="E175"/>
       <c r="F175" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="G175" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -6166,16 +6439,16 @@
         <v>18</v>
       </c>
       <c r="D176" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="E176" t="s">
         <v>670</v>
       </c>
       <c r="F176" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="G176" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -6189,16 +6462,16 @@
         <v>26</v>
       </c>
       <c r="D177" t="s">
-        <v>778</v>
+        <v>768</v>
       </c>
       <c r="E177" t="s">
-        <v>779</v>
+        <v>769</v>
       </c>
       <c r="F177" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="G177" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -6281,7 +6554,7 @@
         <v>634</v>
       </c>
       <c r="G183" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -6299,7 +6572,7 @@
         <v>634</v>
       </c>
       <c r="G184" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -6317,7 +6590,7 @@
         <v>634</v>
       </c>
       <c r="G185" s="17" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
@@ -6325,7 +6598,7 @@
         <v>585</v>
       </c>
       <c r="B186" t="s">
-        <v>771</v>
+        <v>761</v>
       </c>
       <c r="C186" s="11">
         <v>23</v>
@@ -6335,7 +6608,7 @@
         <v>634</v>
       </c>
       <c r="G186" s="17" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -6353,7 +6626,7 @@
         <v>634</v>
       </c>
       <c r="G187" s="17" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
@@ -6474,10 +6747,10 @@
         <v>8</v>
       </c>
       <c r="D197" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="G197" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
@@ -6491,10 +6764,10 @@
         <v>116</v>
       </c>
       <c r="D198" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="G198" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
       <c r="I198" t="s">
         <v>123</v>
@@ -6514,7 +6787,7 @@
         <v>19</v>
       </c>
       <c r="D199" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
@@ -6528,13 +6801,13 @@
         <v>74</v>
       </c>
       <c r="D200" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>644</v>
       </c>
       <c r="G200" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
@@ -6548,13 +6821,13 @@
         <v>192</v>
       </c>
       <c r="D201" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="G201" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="I201" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="J201" s="7" t="s">
         <v>122</v>
@@ -6571,10 +6844,10 @@
         <v>231</v>
       </c>
       <c r="D202" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="G202" t="s">
-        <v>785</v>
+        <v>775</v>
       </c>
       <c r="I202" t="s">
         <v>119</v>
@@ -6594,13 +6867,13 @@
         <v>23</v>
       </c>
       <c r="D203" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G203" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
@@ -6614,10 +6887,10 @@
         <v>6</v>
       </c>
       <c r="D204" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="G204" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
@@ -6631,10 +6904,10 @@
         <v>4</v>
       </c>
       <c r="D205" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
       <c r="G205" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
     </row>
     <row r="210" spans="2:10" x14ac:dyDescent="0.2">
@@ -7021,7 +7294,7 @@
       <c r="B257" t="s">
         <v>451</v>
       </c>
-      <c r="C257" s="10">
+      <c r="C257" s="23">
         <v>3</v>
       </c>
       <c r="D257" t="s">
@@ -7031,6 +7304,9 @@
       <c r="F257" t="s">
         <v>618</v>
       </c>
+      <c r="G257" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
@@ -7039,14 +7315,21 @@
       <c r="B258" t="s">
         <v>453</v>
       </c>
-      <c r="C258" s="10">
+      <c r="C258" s="29">
         <v>18</v>
       </c>
       <c r="D258" t="s">
         <v>619</v>
       </c>
-      <c r="E258"/>
-      <c r="F258"/>
+      <c r="E258" t="s">
+        <v>844</v>
+      </c>
+      <c r="F258" t="s">
+        <v>618</v>
+      </c>
+      <c r="G258" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
@@ -7055,14 +7338,21 @@
       <c r="B259" t="s">
         <v>455</v>
       </c>
-      <c r="C259" s="10">
+      <c r="C259" s="29">
         <v>4</v>
       </c>
       <c r="D259" t="s">
         <v>619</v>
       </c>
-      <c r="E259"/>
-      <c r="F259"/>
+      <c r="E259" t="s">
+        <v>843</v>
+      </c>
+      <c r="F259" t="s">
+        <v>618</v>
+      </c>
+      <c r="G259" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
@@ -7071,14 +7361,21 @@
       <c r="B260" t="s">
         <v>457</v>
       </c>
-      <c r="C260" s="10">
+      <c r="C260" s="29">
         <v>10</v>
       </c>
       <c r="D260" t="s">
         <v>619</v>
       </c>
-      <c r="E260"/>
-      <c r="F260"/>
+      <c r="E260" t="s">
+        <v>842</v>
+      </c>
+      <c r="F260" t="s">
+        <v>618</v>
+      </c>
+      <c r="G260" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
@@ -7093,24 +7390,38 @@
       <c r="D261" t="s">
         <v>619</v>
       </c>
-      <c r="E261"/>
-      <c r="F261"/>
+      <c r="E261" t="s">
+        <v>686</v>
+      </c>
+      <c r="F261" t="s">
+        <v>618</v>
+      </c>
+      <c r="G261" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>460</v>
       </c>
       <c r="B262" t="s">
-        <v>461</v>
-      </c>
-      <c r="C262" s="10">
+        <v>833</v>
+      </c>
+      <c r="C262" s="23">
         <v>14</v>
       </c>
       <c r="D262" t="s">
         <v>619</v>
       </c>
-      <c r="E262"/>
-      <c r="F262"/>
+      <c r="E262" t="s">
+        <v>834</v>
+      </c>
+      <c r="F262" t="s">
+        <v>618</v>
+      </c>
+      <c r="G262" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
@@ -7119,14 +7430,21 @@
       <c r="B263" t="s">
         <v>461</v>
       </c>
-      <c r="C263" s="10">
+      <c r="C263" s="23">
         <v>23</v>
       </c>
       <c r="D263" t="s">
         <v>619</v>
       </c>
-      <c r="E263"/>
-      <c r="F263"/>
+      <c r="E263" t="s">
+        <v>836</v>
+      </c>
+      <c r="F263" t="s">
+        <v>618</v>
+      </c>
+      <c r="G263" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
@@ -7135,14 +7453,21 @@
       <c r="B264" t="s">
         <v>464</v>
       </c>
-      <c r="C264" s="10">
+      <c r="C264" s="23">
         <v>2</v>
       </c>
       <c r="D264" t="s">
         <v>619</v>
       </c>
-      <c r="E264"/>
-      <c r="F264"/>
+      <c r="E264" t="s">
+        <v>837</v>
+      </c>
+      <c r="F264" t="s">
+        <v>618</v>
+      </c>
+      <c r="G264" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
@@ -7151,14 +7476,21 @@
       <c r="B265" t="s">
         <v>466</v>
       </c>
-      <c r="C265" s="10">
+      <c r="C265" s="23">
         <v>2</v>
       </c>
       <c r="D265" t="s">
         <v>619</v>
       </c>
-      <c r="E265"/>
-      <c r="F265"/>
+      <c r="E265" t="s">
+        <v>840</v>
+      </c>
+      <c r="F265" t="s">
+        <v>618</v>
+      </c>
+      <c r="G265" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
@@ -7255,9 +7587,13 @@
       <c r="D276" t="s">
         <v>616</v>
       </c>
-      <c r="E276"/>
+      <c r="E276" t="s">
+        <v>864</v>
+      </c>
       <c r="F276"/>
-      <c r="G276" s="8"/>
+      <c r="G276" s="8" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
@@ -7272,8 +7608,13 @@
       <c r="D277" t="s">
         <v>616</v>
       </c>
-      <c r="E277"/>
+      <c r="E277" t="s">
+        <v>865</v>
+      </c>
       <c r="F277"/>
+      <c r="G277" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
@@ -8052,7 +8393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D23DC3C-FC33-C942-8382-35514D36DECE}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -8067,115 +8408,115 @@
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>790</v>
+        <v>780</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
       <c r="B4" t="s">
-        <v>799</v>
+        <v>789</v>
       </c>
       <c r="C4" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="D4" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="E4" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="B6" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="C6" t="s">
-        <v>806</v>
+        <v>796</v>
       </c>
       <c r="D6" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="E6" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="B7" t="s">
-        <v>807</v>
+        <v>797</v>
       </c>
       <c r="C7" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="E7" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>784</v>
+      </c>
+      <c r="B8" t="s">
         <v>794</v>
       </c>
-      <c r="B8" t="s">
-        <v>804</v>
-      </c>
       <c r="C8" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="E8" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="B9" t="s">
-        <v>800</v>
+        <v>790</v>
       </c>
       <c r="C9" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="E9" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="B10" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C10" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E10" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="B11" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="C11" t="s">
-        <v>798</v>
+        <v>788</v>
       </c>
       <c r="D11" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="E11" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -8195,40 +8536,40 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="C5" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
     </row>
   </sheetData>
@@ -8241,38 +8582,38 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="C4" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="C5" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="C6" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -8281,6 +8622,98 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84233AF-9805-0746-902B-2057B627BF11}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>810</v>
+      </c>
+      <c r="C3" t="s">
+        <v>876</v>
+      </c>
+      <c r="D3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>870</v>
+      </c>
+      <c r="C4" t="s">
+        <v>878</v>
+      </c>
+      <c r="D4" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>869</v>
+      </c>
+      <c r="C5" t="s">
+        <v>880</v>
+      </c>
+      <c r="D5" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>871</v>
+      </c>
+      <c r="C6" t="s">
+        <v>882</v>
+      </c>
+      <c r="D6" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>875</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A29F90F-24B9-3647-BF97-D46598CD3CE5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -8292,7 +8725,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -8300,7 +8733,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -8308,7 +8741,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -8316,7 +8749,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -8324,7 +8757,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -8332,7 +8765,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -8340,7 +8773,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -8348,7 +8781,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -8356,12 +8789,12 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vorbereitungen für ABSIS Platinen Bestellung
</commit_message>
<xml_diff>
--- a/Metric Modifications/Replacement_COTS.xlsx
+++ b/Metric Modifications/Replacement_COTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/home/github/OpenHornet-metric/Metric Modifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D320122-BE65-8443-960C-B204F3208D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC227F55-F73B-8340-8F9E-8C1FC9C3DBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" xr2:uid="{D93EFF7A-6B33-AC4D-9A9C-C443CD52EB89}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="900">
   <si>
     <t>M4 x 30 mm</t>
   </si>
@@ -2659,12 +2659,6 @@
     <t>M2 x 5 mm</t>
   </si>
   <si>
-    <t>2,1844 mm x 9,525 mm</t>
-  </si>
-  <si>
-    <t>2,1844 mm x 38,1 mm</t>
-  </si>
-  <si>
     <t>M2 x 40 mm</t>
   </si>
   <si>
@@ -2717,6 +2711,60 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 38,1 mm, Außen 4,76 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 9,525 mm, Außen 3,175 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 9,525 mm, Außen 4,76 mm</t>
+  </si>
+  <si>
+    <t>2,1844 mm x 25,4 mm, Außen 4,76 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 22,225 mm, Außen 6,35 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 63,5 mm, Außen 6,35 mm</t>
+  </si>
+  <si>
+    <t>2,845 mm x 25,4 mm, Außen 4,76 mm</t>
+  </si>
+  <si>
+    <t>M3 x 63 mm</t>
+  </si>
+  <si>
+    <t>3,505 mm x 22,225 mm, Außen 6,35</t>
+  </si>
+  <si>
+    <t>3,505 mm x 38,1 mm, Außen 6,35</t>
+  </si>
+  <si>
+    <t>3,505 mm x 25,4 mm, Außen 6,35</t>
+  </si>
+  <si>
+    <t>4,166 mm x 25,4 mm, Außen 6,35 mm</t>
+  </si>
+  <si>
+    <t>Distanzhülse, Sechskant, weiblich-weiblich, Stahl</t>
+  </si>
+  <si>
+    <t>Distanzhülse, rund, weiblich-weiblich</t>
+  </si>
+  <si>
+    <t>4,826 mm x 101,6 mm</t>
+  </si>
+  <si>
+    <t>M5 x 100 mm</t>
+  </si>
+  <si>
+    <t>4,826 mm x 88,9 mm</t>
+  </si>
+  <si>
+    <t>M5 x 90 mm</t>
   </si>
 </sst>
 </file>
@@ -3369,10 +3417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B20728A-6C41-1849-BB83-42D2A465FBDB}">
-  <dimension ref="A1:J311"/>
+  <dimension ref="A1:J326"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6108,7 +6156,7 @@
         <v>629</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="G157" t="s">
         <v>755</v>
@@ -7578,7 +7626,7 @@
       <c r="A276" t="s">
         <v>509</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B276" s="24" t="s">
         <v>510</v>
       </c>
       <c r="C276" s="10">
@@ -7588,7 +7636,7 @@
         <v>616</v>
       </c>
       <c r="E276" t="s">
-        <v>864</v>
+        <v>883</v>
       </c>
       <c r="F276"/>
       <c r="G276" s="8" t="s">
@@ -7599,7 +7647,7 @@
       <c r="A277" t="s">
         <v>511</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B277" s="24" t="s">
         <v>512</v>
       </c>
       <c r="C277" s="10">
@@ -7609,242 +7657,240 @@
         <v>616</v>
       </c>
       <c r="E277" t="s">
-        <v>865</v>
+        <v>882</v>
       </c>
       <c r="F277"/>
       <c r="G277" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>513</v>
-      </c>
-      <c r="B278" t="s">
-        <v>514</v>
+        <v>515</v>
+      </c>
+      <c r="B278" s="24" t="s">
+        <v>516</v>
       </c>
       <c r="C278" s="10">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D278" t="s">
         <v>616</v>
       </c>
-      <c r="E278"/>
+      <c r="E278" t="s">
+        <v>884</v>
+      </c>
       <c r="F278"/>
+      <c r="G278" s="8" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>515</v>
-      </c>
-      <c r="B279" t="s">
-        <v>516</v>
+        <v>517</v>
+      </c>
+      <c r="B279" s="24" t="s">
+        <v>518</v>
       </c>
       <c r="C279" s="10">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="D279" t="s">
         <v>616</v>
       </c>
-      <c r="E279"/>
+      <c r="E279" t="s">
+        <v>885</v>
+      </c>
       <c r="F279"/>
+      <c r="G279" s="8" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>517</v>
-      </c>
-      <c r="B280" t="s">
-        <v>518</v>
+        <v>533</v>
+      </c>
+      <c r="B280" s="24" t="s">
+        <v>124</v>
       </c>
       <c r="C280" s="10">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D280" t="s">
-        <v>616</v>
-      </c>
-      <c r="E280"/>
+        <v>617</v>
+      </c>
+      <c r="E280" t="s">
+        <v>884</v>
+      </c>
       <c r="F280"/>
+      <c r="G280" s="8" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>519</v>
-      </c>
-      <c r="B281" t="s">
-        <v>520</v>
+        <v>534</v>
+      </c>
+      <c r="B281" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="C281" s="10">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D281" t="s">
-        <v>616</v>
-      </c>
-      <c r="E281"/>
+        <v>617</v>
+      </c>
+      <c r="E281" t="s">
+        <v>885</v>
+      </c>
       <c r="F281"/>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A282" t="s">
-        <v>521</v>
-      </c>
-      <c r="B282" t="s">
-        <v>522</v>
-      </c>
-      <c r="C282" s="10">
-        <v>28</v>
-      </c>
-      <c r="D282" t="s">
-        <v>616</v>
-      </c>
-      <c r="E282"/>
-      <c r="F282"/>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>523</v>
-      </c>
-      <c r="B283" t="s">
-        <v>524</v>
+        <v>525</v>
+      </c>
+      <c r="B283" s="24" t="s">
+        <v>526</v>
       </c>
       <c r="C283" s="10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D283" t="s">
-        <v>616</v>
-      </c>
-      <c r="E283"/>
+        <v>895</v>
+      </c>
+      <c r="E283" t="s">
+        <v>886</v>
+      </c>
       <c r="F283"/>
+      <c r="G283" s="8" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>525</v>
-      </c>
-      <c r="B284" t="s">
-        <v>526</v>
+        <v>531</v>
+      </c>
+      <c r="B284" s="24" t="s">
+        <v>532</v>
       </c>
       <c r="C284" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D284" t="s">
-        <v>616</v>
-      </c>
-      <c r="E284"/>
+        <v>617</v>
+      </c>
+      <c r="E284" t="s">
+        <v>888</v>
+      </c>
       <c r="F284"/>
+      <c r="G284" s="8" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>527</v>
-      </c>
-      <c r="B285" t="s">
-        <v>528</v>
+        <v>513</v>
+      </c>
+      <c r="B285" s="24" t="s">
+        <v>514</v>
       </c>
       <c r="C285" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D285" t="s">
         <v>616</v>
       </c>
-      <c r="E285"/>
+      <c r="E285" t="s">
+        <v>887</v>
+      </c>
       <c r="F285"/>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A286" t="s">
-        <v>529</v>
-      </c>
-      <c r="B286" t="s">
-        <v>530</v>
-      </c>
-      <c r="C286" s="10">
-        <v>1</v>
-      </c>
-      <c r="D286" t="s">
-        <v>616</v>
-      </c>
-      <c r="E286"/>
-      <c r="F286"/>
+      <c r="G285" s="8" t="s">
+        <v>889</v>
+      </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>531</v>
-      </c>
-      <c r="B287" t="s">
-        <v>532</v>
+        <v>519</v>
+      </c>
+      <c r="B287" s="24" t="s">
+        <v>520</v>
       </c>
       <c r="C287" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D287" t="s">
-        <v>617</v>
-      </c>
-      <c r="E287"/>
+        <v>616</v>
+      </c>
+      <c r="E287" t="s">
+        <v>890</v>
+      </c>
       <c r="F287"/>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>533</v>
-      </c>
-      <c r="B288" t="s">
-        <v>124</v>
+        <v>521</v>
+      </c>
+      <c r="B288" s="24" t="s">
+        <v>522</v>
       </c>
       <c r="C288" s="10">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D288" t="s">
-        <v>617</v>
-      </c>
-      <c r="E288"/>
+        <v>616</v>
+      </c>
+      <c r="E288" t="s">
+        <v>891</v>
+      </c>
       <c r="F288"/>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>534</v>
-      </c>
-      <c r="B289" t="s">
-        <v>125</v>
+        <v>535</v>
+      </c>
+      <c r="B289" s="24" t="s">
+        <v>536</v>
       </c>
       <c r="C289" s="10">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D289" t="s">
         <v>617</v>
       </c>
-      <c r="E289"/>
+      <c r="E289" t="s">
+        <v>890</v>
+      </c>
       <c r="F289"/>
+      <c r="G289" s="8" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>535</v>
-      </c>
-      <c r="B290" t="s">
-        <v>536</v>
+        <v>537</v>
+      </c>
+      <c r="B290" s="24" t="s">
+        <v>538</v>
       </c>
       <c r="C290" s="10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D290" t="s">
         <v>617</v>
       </c>
-      <c r="E290"/>
+      <c r="E290" t="s">
+        <v>892</v>
+      </c>
       <c r="F290"/>
-    </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
-        <v>537</v>
-      </c>
-      <c r="B291" t="s">
-        <v>538</v>
-      </c>
-      <c r="C291" s="10">
-        <v>12</v>
-      </c>
-      <c r="D291" t="s">
-        <v>617</v>
-      </c>
-      <c r="E291"/>
-      <c r="F291"/>
+      <c r="G290" s="8" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>539</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B292" s="24" t="s">
         <v>540</v>
       </c>
       <c r="C292" s="10">
@@ -7853,184 +7899,247 @@
       <c r="D292" t="s">
         <v>617</v>
       </c>
-      <c r="E292"/>
+      <c r="E292" t="s">
+        <v>893</v>
+      </c>
       <c r="F292"/>
+      <c r="G292" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>541</v>
-      </c>
-      <c r="B294" t="s">
-        <v>542</v>
+        <v>527</v>
+      </c>
+      <c r="B294" s="24" t="s">
+        <v>528</v>
       </c>
       <c r="C294" s="10">
-        <v>28</v>
-      </c>
-      <c r="E294"/>
+        <v>1</v>
+      </c>
+      <c r="D294" t="s">
+        <v>895</v>
+      </c>
+      <c r="E294" t="s">
+        <v>898</v>
+      </c>
       <c r="F294"/>
-      <c r="G294" s="8"/>
+      <c r="G294" t="s">
+        <v>899</v>
+      </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>543</v>
-      </c>
-      <c r="B295" t="s">
-        <v>544</v>
+        <v>529</v>
+      </c>
+      <c r="B295" s="24" t="s">
+        <v>530</v>
       </c>
       <c r="C295" s="10">
-        <v>10</v>
-      </c>
-      <c r="E295"/>
+        <v>1</v>
+      </c>
+      <c r="D295" t="s">
+        <v>895</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>896</v>
+      </c>
       <c r="F295"/>
-    </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A296" t="s">
-        <v>545</v>
-      </c>
-      <c r="B296" t="s">
-        <v>546</v>
-      </c>
-      <c r="C296" s="10">
-        <v>1</v>
-      </c>
-      <c r="E296"/>
-      <c r="F296"/>
+      <c r="G295" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>547</v>
-      </c>
-      <c r="B297" t="s">
-        <v>548</v>
+        <v>523</v>
+      </c>
+      <c r="B297" s="24" t="s">
+        <v>524</v>
       </c>
       <c r="C297" s="10">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="D297" t="s">
+        <v>894</v>
       </c>
       <c r="E297"/>
       <c r="F297"/>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A300" t="s">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>541</v>
+      </c>
+      <c r="B309" t="s">
+        <v>542</v>
+      </c>
+      <c r="C309" s="10">
+        <v>28</v>
+      </c>
+      <c r="E309"/>
+      <c r="F309"/>
+      <c r="G309" s="8"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>543</v>
+      </c>
+      <c r="B310" t="s">
+        <v>544</v>
+      </c>
+      <c r="C310" s="10">
+        <v>10</v>
+      </c>
+      <c r="E310"/>
+      <c r="F310"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>545</v>
+      </c>
+      <c r="B311" t="s">
+        <v>546</v>
+      </c>
+      <c r="C311" s="10">
+        <v>1</v>
+      </c>
+      <c r="E311"/>
+      <c r="F311"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>547</v>
+      </c>
+      <c r="B312" t="s">
+        <v>548</v>
+      </c>
+      <c r="C312" s="10">
+        <v>3</v>
+      </c>
+      <c r="E312"/>
+      <c r="F312"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
         <v>600</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B315" t="s">
         <v>601</v>
       </c>
-      <c r="C300" s="10">
+      <c r="C315" s="10">
         <v>1</v>
       </c>
-      <c r="E300"/>
-      <c r="F300"/>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A301" t="s">
+      <c r="E315"/>
+      <c r="F315"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
         <v>602</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B316" t="s">
         <v>603</v>
       </c>
-      <c r="C301" s="10">
+      <c r="C316" s="10">
         <v>2</v>
       </c>
-      <c r="E301"/>
-      <c r="F301"/>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A302" t="s">
+      <c r="E316"/>
+      <c r="F316"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
         <v>604</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B317" t="s">
         <v>605</v>
       </c>
-      <c r="C302" s="10">
+      <c r="C317" s="10">
         <v>28</v>
       </c>
-      <c r="E302"/>
-      <c r="F302"/>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A304" s="9" t="s">
+      <c r="E317"/>
+      <c r="F317"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A319" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B319" t="s">
         <v>420</v>
       </c>
-      <c r="C304" s="10">
+      <c r="C319" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A305" s="9" t="s">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A320" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B320" t="s">
         <v>422</v>
       </c>
-      <c r="C305" s="10">
+      <c r="C320" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A306" s="9" t="s">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B321" t="s">
         <v>424</v>
       </c>
-      <c r="C306" s="10">
+      <c r="C321" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A307" s="9" t="s">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B322" t="s">
         <v>426</v>
       </c>
-      <c r="C307" s="10">
+      <c r="C322" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A308" s="9" t="s">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B323" t="s">
         <v>428</v>
       </c>
-      <c r="C308" s="10">
+      <c r="C323" s="10">
         <v>64</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A309" s="13" t="s">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B324" t="s">
         <v>430</v>
       </c>
-      <c r="C309" s="10">
+      <c r="C324" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A310" s="9"/>
-      <c r="B310" t="s">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325" s="9"/>
+      <c r="B325" t="s">
         <v>431</v>
       </c>
-      <c r="C310" s="10">
+      <c r="C325" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A311" s="9" t="s">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B326" t="s">
         <v>433</v>
       </c>
-      <c r="C311" s="10">
+      <c r="C326" s="10">
         <v>2</v>
       </c>
     </row>
@@ -8636,7 +8745,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8644,53 +8753,53 @@
         <v>810</v>
       </c>
       <c r="C3" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C4" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D4" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C5" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D5" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C6" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D6" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8700,12 +8809,12 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>